<commit_message>
configuracion area 1 ospf
</commit_message>
<xml_diff>
--- a/docs/dhcp_pool.xlsx
+++ b/docs/dhcp_pool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna3-mj10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB52AAA8-4BC5-434B-BFDF-A708867D89A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C06F3F-8A8B-4B0B-81EB-8BE04A256B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{86C8F174-9649-4CB1-8963-47518D3DEE91}"/>
+    <workbookView minimized="1" xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{86C8F174-9649-4CB1-8963-47518D3DEE91}"/>
   </bookViews>
   <sheets>
     <sheet name="DHCP" sheetId="1" r:id="rId1"/>
@@ -132,28 +132,28 @@
     <t>dom NET-12</t>
   </si>
   <si>
-    <t>IP DH EX ADD 192.168.0.0 192.168.0.5</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.32 192.168.0.37</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.64 192.168.0.69</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.96 192.168.0.101</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.128 192.168.0.133</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.160 192.168.0.165</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.192 192.168.0.197</t>
-  </si>
-  <si>
-    <t>IP DH EX ADD 192.168.0.224 192.168.0.229</t>
+    <t>IP DH EX 192.168.0.0 192.168.0.5</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.32 192.168.0.37</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.64 192.168.0.69</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.96 192.168.0.101</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.128 192.168.0.133</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.160 192.168.0.165</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.192 192.168.0.197</t>
+  </si>
+  <si>
+    <t>IP DH EX  192.168.0.224 192.168.0.229</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:A49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A49"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>